<commit_message>
fix league pc text
</commit_message>
<xml_diff>
--- a/xlsx/data.xlsx
+++ b/xlsx/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tom/Developer/PKMN_G1/pokeredCHS/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BB3139D-7155-7D47-8053-55092A75CE45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{161E2EC6-84FA-F04F-8A03-CBF01510D83D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20480" activeTab="6" xr2:uid="{5D9A02DE-DD85-974B-B8A1-A92382739B9C}"/>
   </bookViews>
@@ -6837,10 +6837,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>恭喜登入名人堂  第@</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>恭喜登入名人堂！@</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -7548,6 +7544,10 @@
   </si>
   <si>
     <t>v110@</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 第   次 登入名人堂@</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -11544,7 +11544,7 @@
         <v>620</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>2128</v>
+        <v>2127</v>
       </c>
     </row>
     <row r="94" spans="2:3">
@@ -14084,7 +14084,7 @@
     </row>
     <row r="13" spans="1:8">
       <c r="B13" s="1" t="s">
-        <v>2051</v>
+        <v>2050</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>1260</v>
@@ -14164,7 +14164,7 @@
     </row>
     <row r="23" spans="2:8">
       <c r="F23" s="1" t="s">
-        <v>2052</v>
+        <v>2051</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>1260</v>
@@ -14175,7 +14175,7 @@
         <v>1239</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="25" spans="2:8">
@@ -14183,7 +14183,7 @@
         <v>1240</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="26" spans="2:8">
@@ -14201,7 +14201,7 @@
         <v>1243</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="29" spans="2:8">
@@ -14219,7 +14219,7 @@
         <v>1246</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="32" spans="2:8">
@@ -14227,7 +14227,7 @@
         <v>1247</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="33" spans="1:18">
@@ -14235,7 +14235,7 @@
         <v>1248</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="34" spans="1:18">
@@ -14243,12 +14243,12 @@
         <v>1249</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="35" spans="1:18">
       <c r="B35" s="6" t="s">
-        <v>2143</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="36" spans="1:18">
@@ -14256,7 +14256,7 @@
         <v>1251</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="37" spans="1:18">
@@ -14264,7 +14264,7 @@
         <v>1248</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="38" spans="1:18">
@@ -14272,7 +14272,7 @@
         <v>1252</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>2040</v>
+        <v>2039</v>
       </c>
     </row>
     <row r="39" spans="1:18">
@@ -14280,12 +14280,12 @@
         <v>1253</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="40" spans="1:18">
       <c r="B40" s="6" t="s">
-        <v>2048</v>
+        <v>2047</v>
       </c>
     </row>
     <row r="41" spans="1:18">
@@ -14293,7 +14293,7 @@
         <v>1255</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="42" spans="1:18">
@@ -14301,7 +14301,7 @@
         <v>1256</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="43" spans="1:18">
@@ -14309,7 +14309,7 @@
         <v>1257</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>2044</v>
+        <v>2043</v>
       </c>
     </row>
     <row r="44" spans="1:18">
@@ -14317,12 +14317,12 @@
         <v>1258</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>2046</v>
+        <v>2045</v>
       </c>
     </row>
     <row r="45" spans="1:18">
       <c r="B45" s="6" t="s">
-        <v>2049</v>
+        <v>2048</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>1456</v>
@@ -14356,16 +14356,16 @@
         <v>1154</v>
       </c>
       <c r="O47" s="4" t="s">
-        <v>2055</v>
+        <v>2054</v>
       </c>
       <c r="P47" s="8" t="s">
-        <v>2099</v>
+        <v>2098</v>
       </c>
       <c r="Q47" s="1" t="s">
         <v>1155</v>
       </c>
       <c r="R47" s="1" t="s">
-        <v>2024</v>
+        <v>2023</v>
       </c>
     </row>
     <row r="48" spans="1:18">
@@ -14373,7 +14373,7 @@
         <v>1156</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>2025</v>
+        <v>2024</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>1725</v>
@@ -14388,16 +14388,16 @@
         <v>1156</v>
       </c>
       <c r="O48" s="4" t="s">
-        <v>2056</v>
+        <v>2055</v>
       </c>
       <c r="P48" s="8" t="s">
-        <v>2100</v>
+        <v>2099</v>
       </c>
       <c r="Q48" s="1" t="s">
         <v>1157</v>
       </c>
       <c r="R48" s="1" t="s">
-        <v>2026</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="49" spans="2:18">
@@ -14420,10 +14420,10 @@
         <v>1158</v>
       </c>
       <c r="O49" s="4" t="s">
-        <v>2057</v>
+        <v>2056</v>
       </c>
       <c r="P49" s="8" t="s">
-        <v>2101</v>
+        <v>2100</v>
       </c>
       <c r="Q49" s="10" t="s">
         <v>1723</v>
@@ -14449,7 +14449,7 @@
         <v>1159</v>
       </c>
       <c r="O50" s="4" t="s">
-        <v>2058</v>
+        <v>2057</v>
       </c>
       <c r="Q50" s="1" t="s">
         <v>1160</v>
@@ -14460,7 +14460,7 @@
         <v>1161</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>1728</v>
@@ -14475,13 +14475,13 @@
         <v>1161</v>
       </c>
       <c r="O51" s="4" t="s">
-        <v>2059</v>
+        <v>2058</v>
       </c>
       <c r="P51" s="8" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="Q51" s="10" t="s">
-        <v>2054</v>
+        <v>2053</v>
       </c>
     </row>
     <row r="52" spans="2:18">
@@ -14489,7 +14489,7 @@
         <v>1162</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>1729</v>
@@ -14504,16 +14504,16 @@
         <v>1162</v>
       </c>
       <c r="O52" s="4" t="s">
-        <v>2060</v>
+        <v>2059</v>
       </c>
       <c r="P52" s="8" t="s">
-        <v>2113</v>
+        <v>2112</v>
       </c>
       <c r="Q52" s="1" t="s">
         <v>1980</v>
       </c>
       <c r="R52" s="1" t="s">
-        <v>2047</v>
+        <v>2046</v>
       </c>
     </row>
     <row r="53" spans="2:18">
@@ -14521,7 +14521,7 @@
         <v>1163</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>1730</v>
@@ -14536,13 +14536,13 @@
         <v>1163</v>
       </c>
       <c r="O53" s="4" t="s">
-        <v>2061</v>
+        <v>2060</v>
       </c>
       <c r="P53" s="8" t="s">
-        <v>2114</v>
+        <v>2113</v>
       </c>
       <c r="Q53" s="10" t="s">
-        <v>2027</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="54" spans="2:18">
@@ -14565,13 +14565,13 @@
         <v>1164</v>
       </c>
       <c r="O54" s="4" t="s">
-        <v>2062</v>
+        <v>2061</v>
       </c>
       <c r="P54" s="8" t="s">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="Q54" s="10" t="s">
-        <v>2123</v>
+        <v>2122</v>
       </c>
     </row>
     <row r="55" spans="2:18">
@@ -14594,7 +14594,7 @@
         <v>1166</v>
       </c>
       <c r="O55" s="4" t="s">
-        <v>2063</v>
+        <v>2062</v>
       </c>
       <c r="Q55" s="1" t="s">
         <v>1167</v>
@@ -14620,7 +14620,7 @@
         <v>1168</v>
       </c>
       <c r="O56" s="4" t="s">
-        <v>2064</v>
+        <v>2063</v>
       </c>
       <c r="Q56" s="1" t="s">
         <v>1169</v>
@@ -14631,7 +14631,7 @@
         <v>1170</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>2028</v>
+        <v>2027</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>1734</v>
@@ -14646,16 +14646,16 @@
         <v>1170</v>
       </c>
       <c r="O57" s="4" t="s">
-        <v>2065</v>
+        <v>2064</v>
       </c>
       <c r="P57" s="8" t="s">
-        <v>2116</v>
+        <v>2115</v>
       </c>
       <c r="Q57" s="1" t="s">
         <v>1171</v>
       </c>
       <c r="R57" s="1" t="s">
-        <v>2029</v>
+        <v>2028</v>
       </c>
     </row>
     <row r="58" spans="2:18">
@@ -14663,7 +14663,7 @@
         <v>1172</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>2030</v>
+        <v>2029</v>
       </c>
       <c r="G58" s="1" t="s">
         <v>1735</v>
@@ -14678,16 +14678,16 @@
         <v>1172</v>
       </c>
       <c r="O58" s="4" t="s">
-        <v>2066</v>
+        <v>2065</v>
       </c>
       <c r="P58" s="8" t="s">
-        <v>2117</v>
+        <v>2116</v>
       </c>
       <c r="Q58" s="1" t="s">
         <v>1173</v>
       </c>
       <c r="R58" s="1" t="s">
-        <v>2120</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="59" spans="2:18">
@@ -14695,7 +14695,7 @@
         <v>1174</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>2031</v>
+        <v>2030</v>
       </c>
       <c r="G59" s="1" t="s">
         <v>1736</v>
@@ -14710,16 +14710,16 @@
         <v>1174</v>
       </c>
       <c r="O59" s="4" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="P59" s="9" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
       <c r="Q59" s="1" t="s">
         <v>1175</v>
       </c>
       <c r="R59" s="1" t="s">
-        <v>2032</v>
+        <v>2031</v>
       </c>
     </row>
     <row r="60" spans="2:18">
@@ -14742,7 +14742,7 @@
         <v>1176</v>
       </c>
       <c r="O60" s="4" t="s">
-        <v>2068</v>
+        <v>2067</v>
       </c>
       <c r="Q60" s="1" t="s">
         <v>1177</v>
@@ -14753,7 +14753,7 @@
         <v>1178</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>2033</v>
+        <v>2032</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>1738</v>
@@ -14768,16 +14768,16 @@
         <v>1178</v>
       </c>
       <c r="O61" s="4" t="s">
-        <v>2069</v>
+        <v>2068</v>
       </c>
       <c r="P61" s="8" t="s">
-        <v>2118</v>
+        <v>2117</v>
       </c>
       <c r="Q61" s="1" t="s">
         <v>1179</v>
       </c>
       <c r="R61" s="1" t="s">
-        <v>2034</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="62" spans="2:18">
@@ -14800,7 +14800,7 @@
         <v>1180</v>
       </c>
       <c r="O62" s="4" t="s">
-        <v>2070</v>
+        <v>2069</v>
       </c>
       <c r="Q62" s="1" t="s">
         <v>1181</v>
@@ -14826,7 +14826,7 @@
         <v>1182</v>
       </c>
       <c r="O63" s="4" t="s">
-        <v>2071</v>
+        <v>2070</v>
       </c>
       <c r="Q63" s="1" t="s">
         <v>1183</v>
@@ -14837,7 +14837,7 @@
         <v>1184</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>2035</v>
+        <v>2034</v>
       </c>
       <c r="G64" s="1" t="s">
         <v>1741</v>
@@ -14852,10 +14852,10 @@
         <v>1184</v>
       </c>
       <c r="O64" s="4" t="s">
-        <v>2072</v>
+        <v>2071</v>
       </c>
       <c r="P64" s="4" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="Q64" s="10" t="s">
         <v>1185</v>
@@ -14866,7 +14866,7 @@
         <v>1186</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>1742</v>
@@ -14881,10 +14881,10 @@
         <v>1186</v>
       </c>
       <c r="O65" s="4" t="s">
-        <v>2073</v>
+        <v>2072</v>
       </c>
       <c r="Q65" s="1" t="s">
-        <v>2036</v>
+        <v>2035</v>
       </c>
       <c r="R65" s="7" t="s">
         <v>1456</v>
@@ -14895,7 +14895,7 @@
         <v>1187</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>2037</v>
+        <v>2036</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>1743</v>
@@ -14910,13 +14910,13 @@
         <v>1187</v>
       </c>
       <c r="O66" s="4" t="s">
-        <v>2074</v>
+        <v>2073</v>
       </c>
       <c r="Q66" s="1" t="s">
         <v>1188</v>
       </c>
       <c r="R66" s="1" t="s">
-        <v>2038</v>
+        <v>2037</v>
       </c>
     </row>
     <row r="67" spans="2:18">
@@ -14939,16 +14939,16 @@
         <v>1174</v>
       </c>
       <c r="O67" s="4" t="s">
-        <v>2067</v>
+        <v>2066</v>
       </c>
       <c r="P67" s="4" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="Q67" s="1" t="s">
+        <v>2030</v>
+      </c>
+      <c r="R67" s="1" t="s">
         <v>2031</v>
-      </c>
-      <c r="R67" s="1" t="s">
-        <v>2032</v>
       </c>
     </row>
     <row r="68" spans="2:18">
@@ -14971,7 +14971,7 @@
         <v>1189</v>
       </c>
       <c r="O68" s="4" t="s">
-        <v>2075</v>
+        <v>2074</v>
       </c>
       <c r="Q68" s="1" t="s">
         <v>1190</v>
@@ -14997,7 +14997,7 @@
         <v>1191</v>
       </c>
       <c r="O69" s="4" t="s">
-        <v>2076</v>
+        <v>2075</v>
       </c>
       <c r="Q69" s="1" t="s">
         <v>1192</v>
@@ -15008,7 +15008,7 @@
         <v>1193</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>2039</v>
+        <v>2038</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>1746</v>
@@ -15023,16 +15023,16 @@
         <v>1193</v>
       </c>
       <c r="O70" s="4" t="s">
-        <v>2077</v>
+        <v>2076</v>
       </c>
       <c r="P70" s="4" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="Q70" s="1" t="s">
+        <v>2038</v>
+      </c>
+      <c r="R70" s="1" t="s">
         <v>2039</v>
-      </c>
-      <c r="R70" s="1" t="s">
-        <v>2040</v>
       </c>
     </row>
     <row r="71" spans="2:18">
@@ -15055,7 +15055,7 @@
         <v>1194</v>
       </c>
       <c r="O71" s="4" t="s">
-        <v>2078</v>
+        <v>2077</v>
       </c>
       <c r="Q71" s="1" t="s">
         <v>1195</v>
@@ -15066,7 +15066,7 @@
         <v>1196</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>1748</v>
@@ -15081,16 +15081,16 @@
         <v>1196</v>
       </c>
       <c r="O72" s="4" t="s">
-        <v>2079</v>
+        <v>2078</v>
       </c>
       <c r="P72" s="4" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="Q72" s="1" t="s">
-        <v>2119</v>
+        <v>2118</v>
       </c>
       <c r="R72" s="1" t="s">
-        <v>2050</v>
+        <v>2049</v>
       </c>
     </row>
     <row r="73" spans="2:18">
@@ -15098,7 +15098,7 @@
         <v>1197</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
       <c r="G73" s="1" t="s">
         <v>1749</v>
@@ -15113,13 +15113,13 @@
         <v>1197</v>
       </c>
       <c r="O73" s="4" t="s">
-        <v>2124</v>
+        <v>2123</v>
       </c>
       <c r="P73" s="4" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="Q73" s="10" t="s">
-        <v>2041</v>
+        <v>2040</v>
       </c>
     </row>
     <row r="74" spans="2:18">
@@ -15142,16 +15142,16 @@
         <v>1198</v>
       </c>
       <c r="O74" s="4" t="s">
-        <v>2080</v>
+        <v>2079</v>
       </c>
       <c r="P74" s="4" t="s">
-        <v>2109</v>
+        <v>2108</v>
       </c>
       <c r="Q74" s="1" t="s">
         <v>1998</v>
       </c>
       <c r="R74" s="1" t="s">
-        <v>2042</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="75" spans="2:18">
@@ -15174,7 +15174,7 @@
         <v>1199</v>
       </c>
       <c r="O75" s="4" t="s">
-        <v>2081</v>
+        <v>2080</v>
       </c>
       <c r="Q75" s="1" t="s">
         <v>1200</v>
@@ -15185,7 +15185,7 @@
         <v>1201</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>2043</v>
+        <v>2042</v>
       </c>
       <c r="G76" s="1" t="s">
         <v>1752</v>
@@ -15200,16 +15200,16 @@
         <v>1201</v>
       </c>
       <c r="O76" s="4" t="s">
-        <v>2082</v>
+        <v>2081</v>
       </c>
       <c r="P76" s="4" t="s">
-        <v>2110</v>
+        <v>2109</v>
       </c>
       <c r="Q76" s="1" t="s">
         <v>1202</v>
       </c>
       <c r="R76" s="1" t="s">
-        <v>2053</v>
+        <v>2052</v>
       </c>
     </row>
     <row r="77" spans="2:18">
@@ -15235,16 +15235,16 @@
         <v>1203</v>
       </c>
       <c r="O77" s="4" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="P77" s="4" t="s">
-        <v>2111</v>
+        <v>2110</v>
       </c>
       <c r="Q77" s="1" t="s">
         <v>2002</v>
       </c>
       <c r="R77" s="11" t="s">
-        <v>2121</v>
+        <v>2120</v>
       </c>
     </row>
     <row r="78" spans="2:18">
@@ -15252,7 +15252,7 @@
         <v>1205</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>1206</v>
@@ -15270,16 +15270,16 @@
         <v>1205</v>
       </c>
       <c r="O78" s="4" t="s">
-        <v>2083</v>
+        <v>2082</v>
       </c>
       <c r="P78" s="4" t="s">
-        <v>2112</v>
+        <v>2111</v>
       </c>
       <c r="Q78" s="1" t="s">
-        <v>2045</v>
+        <v>2044</v>
       </c>
       <c r="R78" s="11" t="s">
-        <v>2122</v>
+        <v>2121</v>
       </c>
     </row>
     <row r="79" spans="2:18">
@@ -15305,7 +15305,7 @@
         <v>1207</v>
       </c>
       <c r="O79" s="4" t="s">
-        <v>2084</v>
+        <v>2083</v>
       </c>
     </row>
     <row r="80" spans="2:18">
@@ -15331,7 +15331,7 @@
         <v>1209</v>
       </c>
       <c r="O80" s="4" t="s">
-        <v>2085</v>
+        <v>2084</v>
       </c>
     </row>
     <row r="81" spans="2:15">
@@ -15357,7 +15357,7 @@
         <v>1211</v>
       </c>
       <c r="O81" s="4" t="s">
-        <v>2086</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="82" spans="2:15">
@@ -15383,7 +15383,7 @@
         <v>1213</v>
       </c>
       <c r="O82" s="4" t="s">
-        <v>2087</v>
+        <v>2086</v>
       </c>
     </row>
     <row r="83" spans="2:15">
@@ -15409,7 +15409,7 @@
         <v>1215</v>
       </c>
       <c r="O83" s="4" t="s">
-        <v>2088</v>
+        <v>2087</v>
       </c>
     </row>
     <row r="84" spans="2:15">
@@ -15435,7 +15435,7 @@
         <v>1217</v>
       </c>
       <c r="O84" s="4" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
     </row>
     <row r="85" spans="2:15">
@@ -15461,7 +15461,7 @@
         <v>1219</v>
       </c>
       <c r="O85" s="4" t="s">
-        <v>2090</v>
+        <v>2089</v>
       </c>
     </row>
     <row r="86" spans="2:15">
@@ -15487,7 +15487,7 @@
         <v>1221</v>
       </c>
       <c r="O86" s="4" t="s">
-        <v>2091</v>
+        <v>2090</v>
       </c>
     </row>
     <row r="87" spans="2:15">
@@ -15513,7 +15513,7 @@
         <v>1223</v>
       </c>
       <c r="O87" s="4" t="s">
-        <v>2092</v>
+        <v>2091</v>
       </c>
     </row>
     <row r="88" spans="2:15">
@@ -15539,7 +15539,7 @@
         <v>1225</v>
       </c>
       <c r="O88" s="4" t="s">
-        <v>2093</v>
+        <v>2092</v>
       </c>
     </row>
     <row r="89" spans="2:15">
@@ -15565,7 +15565,7 @@
         <v>1226</v>
       </c>
       <c r="O89" s="4" t="s">
-        <v>2094</v>
+        <v>2093</v>
       </c>
     </row>
     <row r="90" spans="2:15">
@@ -15591,7 +15591,7 @@
         <v>1228</v>
       </c>
       <c r="O90" s="4" t="s">
-        <v>2095</v>
+        <v>2094</v>
       </c>
     </row>
     <row r="91" spans="2:15">
@@ -15617,7 +15617,7 @@
         <v>1230</v>
       </c>
       <c r="O91" s="4" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="92" spans="2:15">
@@ -15643,7 +15643,7 @@
         <v>1232</v>
       </c>
       <c r="O92" s="4" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="93" spans="2:15">
@@ -15669,7 +15669,7 @@
         <v>1234</v>
       </c>
       <c r="O93" s="4" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="94" spans="2:15">
@@ -15711,8 +15711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C9419DE-5B49-5F4A-B230-D7BA1B4ADB25}">
   <dimension ref="A1:J347"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="116" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" topLeftCell="A166" zoomScale="112" zoomScaleNormal="116" workbookViewId="0">
+      <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -15836,7 +15836,7 @@
         <v>1151</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>2137</v>
+        <v>2136</v>
       </c>
       <c r="E14" t="s">
         <v>1303</v>
@@ -15882,26 +15882,26 @@
     </row>
     <row r="19" spans="1:6">
       <c r="B19" t="s">
-        <v>2138</v>
+        <v>2137</v>
       </c>
       <c r="C19" t="s">
-        <v>2141</v>
+        <v>2140</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" t="s">
-        <v>2139</v>
+        <v>2138</v>
       </c>
       <c r="C20" t="s">
-        <v>2142</v>
+        <v>2141</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" t="s">
-        <v>2140</v>
+        <v>2139</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>2175</v>
+        <v>2174</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -16381,10 +16381,10 @@
     </row>
     <row r="80" spans="1:6">
       <c r="B80" t="s">
-        <v>2131</v>
+        <v>2130</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>2129</v>
+        <v>2128</v>
       </c>
       <c r="F80" t="s">
         <v>1858</v>
@@ -16392,15 +16392,15 @@
     </row>
     <row r="81" spans="1:6">
       <c r="B81" t="s">
-        <v>2132</v>
+        <v>2131</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>2130</v>
+        <v>2129</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="B82" t="s">
-        <v>2133</v>
+        <v>2132</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>1864</v>
@@ -16433,15 +16433,15 @@
         <v>1380</v>
       </c>
       <c r="C85" t="s">
+        <v>2133</v>
+      </c>
+      <c r="F85" t="s">
         <v>2134</v>
-      </c>
-      <c r="F85" t="s">
-        <v>2135</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="B86" t="s">
-        <v>2136</v>
+        <v>2135</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>1381</v>
@@ -17234,7 +17234,7 @@
         <v>1514</v>
       </c>
       <c r="C187" t="s">
-        <v>2018</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -17271,7 +17271,7 @@
         <v>1520</v>
       </c>
       <c r="C192" t="s">
-        <v>2017</v>
+        <v>2175</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -18349,7 +18349,7 @@
         <v>1591</v>
       </c>
       <c r="C285" t="s">
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="F285" t="s">
         <v>1593</v>
@@ -18389,7 +18389,7 @@
         <v>1601</v>
       </c>
       <c r="C287" t="s">
-        <v>2022</v>
+        <v>2021</v>
       </c>
       <c r="F287" t="s">
         <v>1603</v>
@@ -18537,7 +18537,7 @@
         <v>1683</v>
       </c>
       <c r="C295" t="s">
-        <v>2144</v>
+        <v>2143</v>
       </c>
       <c r="F295" t="s">
         <v>1684</v>
@@ -18548,7 +18548,7 @@
         <v>1685</v>
       </c>
       <c r="C296" t="s">
-        <v>2145</v>
+        <v>2144</v>
       </c>
       <c r="F296" t="s">
         <v>1686</v>
@@ -18710,7 +18710,7 @@
         <v>1868</v>
       </c>
       <c r="C314" t="s">
-        <v>2127</v>
+        <v>2126</v>
       </c>
     </row>
     <row r="315" spans="1:7">
@@ -18718,7 +18718,7 @@
         <v>1869</v>
       </c>
       <c r="C315" t="s">
-        <v>2126</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="316" spans="1:7">
@@ -18755,7 +18755,7 @@
     </row>
     <row r="320" spans="1:7">
       <c r="A320" t="s">
-        <v>2125</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="321" spans="1:6">
@@ -18795,7 +18795,7 @@
         <v>1916</v>
       </c>
       <c r="C325" t="s">
-        <v>2020</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="326" spans="1:6">
@@ -18803,7 +18803,7 @@
         <v>1918</v>
       </c>
       <c r="C326" t="s">
-        <v>2021</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="327" spans="1:6">
@@ -18877,7 +18877,7 @@
     </row>
     <row r="336" spans="1:6">
       <c r="B336" t="s">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="C336" t="s">
         <v>1938</v>
@@ -19033,7 +19033,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>2146</v>
+        <v>2145</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>449</v>
@@ -19041,26 +19041,26 @@
     </row>
     <row r="5" spans="1:6">
       <c r="B5" s="12" t="s">
+        <v>2146</v>
+      </c>
+      <c r="C5" t="s">
         <v>2147</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2148</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="B6" s="12" t="s">
+        <v>2148</v>
+      </c>
+      <c r="C6" t="s">
         <v>2149</v>
-      </c>
-      <c r="C6" t="s">
-        <v>2150</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="19">
       <c r="B7" s="12" t="s">
-        <v>2152</v>
+        <v>2151</v>
       </c>
       <c r="C7" t="s">
-        <v>2151</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -19070,74 +19070,74 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>2157</v>
+        <v>2156</v>
       </c>
       <c r="F9" t="s">
-        <v>2162</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="B10" s="12" t="s">
-        <v>2171</v>
+        <v>2170</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>2173</v>
+        <v>2172</v>
       </c>
     </row>
     <row r="11" spans="1:6">
       <c r="B11" s="12" t="s">
-        <v>2172</v>
+        <v>2171</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>2174</v>
+        <v>2173</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="B12" s="12" t="s">
+        <v>2157</v>
+      </c>
+      <c r="D12" s="12" t="s">
         <v>2158</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>2159</v>
       </c>
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="12" t="s">
+        <v>2159</v>
+      </c>
+      <c r="D13" s="12" t="s">
         <v>2160</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>2161</v>
       </c>
     </row>
     <row r="14" spans="1:6">
       <c r="B14" s="12" t="s">
+        <v>2162</v>
+      </c>
+      <c r="D14" s="12" t="s">
         <v>2163</v>
-      </c>
-      <c r="D14" s="12" t="s">
-        <v>2164</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="B15" s="12" t="s">
+        <v>2164</v>
+      </c>
+      <c r="D15" s="12" t="s">
         <v>2165</v>
-      </c>
-      <c r="D15" s="12" t="s">
-        <v>2166</v>
       </c>
     </row>
     <row r="16" spans="1:6">
       <c r="B16" s="12" t="s">
+        <v>2166</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>2167</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>2168</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="B17" s="12" t="s">
+        <v>2168</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>2169</v>
-      </c>
-      <c r="D17" s="12" t="s">
-        <v>2170</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -19147,12 +19147,12 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>2153</v>
+        <v>2152</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="B20" s="12" t="s">
-        <v>2154</v>
+        <v>2153</v>
       </c>
       <c r="D20" s="12" t="s">
         <v>1895</v>
@@ -19160,10 +19160,10 @@
     </row>
     <row r="21" spans="1:4">
       <c r="B21" s="12" t="s">
+        <v>2154</v>
+      </c>
+      <c r="D21" s="12" t="s">
         <v>2155</v>
-      </c>
-      <c r="D21" s="12" t="s">
-        <v>2156</v>
       </c>
     </row>
     <row r="22" spans="1:4">

</xml_diff>